<commit_message>
working on new minmal data. fromexcel in minimal case runs, but cognate matching not working yet given minimal excel (not minimal csv files)
</commit_message>
<xml_diff>
--- a/test/data/cldf/new_minimal/minimal.xlsx
+++ b/test/data/cldf/new_minimal/minimal.xlsx
@@ -8,8 +8,6 @@
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
-    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
-    <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
@@ -30,7 +28,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>fictitious!</t>
+          <t>Language comment</t>
         </r>
       </text>
     </comment>
@@ -43,7 +41,20 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>First person singular pronoun as agent of a transitive clause</t>
+          <t>Concept comment</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A3" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Concept comment</t>
         </r>
       </text>
     </comment>
@@ -52,14 +63,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>TG100</t>
   </si>
   <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>Set</t>
   </si>
   <si>
@@ -73,6 +81,15 @@
   </si>
   <si>
     <t>&lt;em&gt; (emphatic) {fict}</t>
+  </si>
+  <si>
+    <t>Woman</t>
+  </si>
+  <si>
+    <t>/am/ (description) {anysource}</t>
+  </si>
+  <si>
+    <t>Person</t>
   </si>
 </sst>
 </file>
@@ -449,10 +466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -462,16 +479,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -479,11 +496,22 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="6" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -491,28 +519,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>